<commit_message>
feat: add 2022-Q1 data
</commit_message>
<xml_diff>
--- a/数据整理/funds/high-score-funds.xlsx
+++ b/数据整理/funds/high-score-funds.xlsx
@@ -12,6 +12,7 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-Q2" sheetId="3" state="visible" r:id="rId3"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-Q3" sheetId="4" state="visible" r:id="rId4"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-Q4" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2022-Q1" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="144525" fullCalcOnLoad="1"/>
@@ -22768,7 +22769,6 @@
           <t>华安香港精选股票(QDII)</t>
         </is>
       </c>
-      <c r="D61" t="inlineStr"/>
       <c r="E61" t="inlineStr">
         <is>
           <t>翁启森</t>
@@ -22833,6 +22833,4930 @@
       <c r="T61" t="inlineStr">
         <is>
           <t>2021-Q4</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:T57"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="6" t="inlineStr">
+        <is>
+          <t>代码</t>
+        </is>
+      </c>
+      <c r="C1" s="6" t="inlineStr">
+        <is>
+          <t>名称</t>
+        </is>
+      </c>
+      <c r="D1" s="6" t="inlineStr">
+        <is>
+          <t>投资风格</t>
+        </is>
+      </c>
+      <c r="E1" s="6" t="inlineStr">
+        <is>
+          <t>基金经理</t>
+        </is>
+      </c>
+      <c r="F1" s="6" t="inlineStr">
+        <is>
+          <t>现任经理管理起始时间</t>
+        </is>
+      </c>
+      <c r="G1" s="6" t="inlineStr">
+        <is>
+          <t>成立时间</t>
+        </is>
+      </c>
+      <c r="H1" s="6" t="inlineStr">
+        <is>
+          <t>三年晨星评级</t>
+        </is>
+      </c>
+      <c r="I1" s="6" t="inlineStr">
+        <is>
+          <t>五年晨星评级</t>
+        </is>
+      </c>
+      <c r="J1" s="6" t="inlineStr">
+        <is>
+          <t>夏普比率</t>
+        </is>
+      </c>
+      <c r="K1" s="6" t="inlineStr">
+        <is>
+          <t>股票仓位</t>
+        </is>
+      </c>
+      <c r="L1" s="6" t="inlineStr">
+        <is>
+          <t>十大持股仓位</t>
+        </is>
+      </c>
+      <c r="M1" s="6" t="inlineStr">
+        <is>
+          <t>两年风险评级</t>
+        </is>
+      </c>
+      <c r="N1" s="6" t="inlineStr">
+        <is>
+          <t>三年风险评级</t>
+        </is>
+      </c>
+      <c r="O1" s="6" t="inlineStr">
+        <is>
+          <t>五年风险评级</t>
+        </is>
+      </c>
+      <c r="P1" s="6" t="inlineStr">
+        <is>
+          <t>阿尔法系数</t>
+        </is>
+      </c>
+      <c r="Q1" s="6" t="inlineStr">
+        <is>
+          <t>贝塔系数</t>
+        </is>
+      </c>
+      <c r="R1" s="6" t="inlineStr">
+        <is>
+          <t>标准差</t>
+        </is>
+      </c>
+      <c r="S1" s="6" t="inlineStr">
+        <is>
+          <t>总资产</t>
+        </is>
+      </c>
+      <c r="T1" s="6" t="inlineStr">
+        <is>
+          <t>数据更新时间</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>161222</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>国投瑞银瑞利灵活配置混合（LOF）</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>大盘价值</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>綦缚鹏</t>
+        </is>
+      </c>
+      <c r="F2" s="8" t="n">
+        <v>42577</v>
+      </c>
+      <c r="G2" s="8" t="n">
+        <v>42587</v>
+      </c>
+      <c r="H2" t="n">
+        <v>5</v>
+      </c>
+      <c r="I2" t="n">
+        <v>5</v>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>2.00</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>63.82</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>25.17</t>
+        </is>
+      </c>
+      <c r="M2" t="n">
+        <v>4</v>
+      </c>
+      <c r="N2" t="n">
+        <v>4</v>
+      </c>
+      <c r="O2" t="n">
+        <v>3</v>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>19.67</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>0.96</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>11.38</t>
+        </is>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>2.21</t>
+        </is>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>2022-Q1</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>519002</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>华安安信消费混合</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>大盘平衡</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>王斌</t>
+        </is>
+      </c>
+      <c r="F3" s="8" t="n">
+        <v>43404</v>
+      </c>
+      <c r="G3" s="8" t="n">
+        <v>41417</v>
+      </c>
+      <c r="H3" t="n">
+        <v>5</v>
+      </c>
+      <c r="I3" t="n">
+        <v>5</v>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>1.89</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>89.00</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>27.51</t>
+        </is>
+      </c>
+      <c r="M3" t="n">
+        <v>3</v>
+      </c>
+      <c r="N3" t="n">
+        <v>4</v>
+      </c>
+      <c r="O3" t="n">
+        <v>3</v>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>30.73</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>0.69</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>19.18</t>
+        </is>
+      </c>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t>80.30</t>
+        </is>
+      </c>
+      <c r="T3" t="inlineStr">
+        <is>
+          <t>2022-Q1</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>001667</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>南方转型增长灵活配置混合</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>大盘平衡</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>林乐峰</t>
+        </is>
+      </c>
+      <c r="F4" s="8" t="n">
+        <v>43084</v>
+      </c>
+      <c r="G4" s="8" t="n">
+        <v>42599</v>
+      </c>
+      <c r="H4" t="n">
+        <v>5</v>
+      </c>
+      <c r="I4" t="n">
+        <v>4</v>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>1.68</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>90.88</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>24.05</t>
+        </is>
+      </c>
+      <c r="M4" t="n">
+        <v>4</v>
+      </c>
+      <c r="N4" t="n">
+        <v>4</v>
+      </c>
+      <c r="O4" t="n">
+        <v>4</v>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>24.06</t>
+        </is>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>0.73</t>
+        </is>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>17.77</t>
+        </is>
+      </c>
+      <c r="S4" t="inlineStr">
+        <is>
+          <t>18.61</t>
+        </is>
+      </c>
+      <c r="T4" t="inlineStr">
+        <is>
+          <t>2022-Q1</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="6" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>673060</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>西部利得景瑞灵活配置混合A</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>大盘成长</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>陈保国</t>
+        </is>
+      </c>
+      <c r="F5" s="8" t="n">
+        <v>43876</v>
+      </c>
+      <c r="G5" s="8" t="n">
+        <v>42607</v>
+      </c>
+      <c r="H5" t="n">
+        <v>5</v>
+      </c>
+      <c r="I5" t="n">
+        <v>5</v>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>1.66</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>91.96</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>33.76</t>
+        </is>
+      </c>
+      <c r="M5" t="n">
+        <v>3</v>
+      </c>
+      <c r="N5" t="n">
+        <v>3</v>
+      </c>
+      <c r="O5" t="n">
+        <v>3</v>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>27.91</t>
+        </is>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>0.60</t>
+        </is>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>19.71</t>
+        </is>
+      </c>
+      <c r="S5" t="inlineStr">
+        <is>
+          <t>10.10</t>
+        </is>
+      </c>
+      <c r="T5" t="inlineStr">
+        <is>
+          <t>2022-Q1</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>519003</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>海富通收益增长混合</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>大盘成长</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>周雪军</t>
+        </is>
+      </c>
+      <c r="F6" s="8" t="n">
+        <v>42164</v>
+      </c>
+      <c r="G6" s="8" t="n">
+        <v>38058</v>
+      </c>
+      <c r="H6" t="n">
+        <v>5</v>
+      </c>
+      <c r="I6" t="n">
+        <v>5</v>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>1.63</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>78.79</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>20.03</t>
+        </is>
+      </c>
+      <c r="M6" t="n">
+        <v>3</v>
+      </c>
+      <c r="N6" t="n">
+        <v>3</v>
+      </c>
+      <c r="O6" t="n">
+        <v>3</v>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>22.43</t>
+        </is>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>1.59</t>
+        </is>
+      </c>
+      <c r="R6" t="inlineStr">
+        <is>
+          <t>16.99</t>
+        </is>
+      </c>
+      <c r="S6" t="inlineStr">
+        <is>
+          <t>35.90</t>
+        </is>
+      </c>
+      <c r="T6" t="inlineStr">
+        <is>
+          <t>2022-Q1</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>750001</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>安信灵活配置混合</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>大盘平衡</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>张竞</t>
+        </is>
+      </c>
+      <c r="F7" s="8" t="n">
+        <v>43098</v>
+      </c>
+      <c r="G7" s="8" t="n">
+        <v>41080</v>
+      </c>
+      <c r="H7" t="n">
+        <v>5</v>
+      </c>
+      <c r="I7" t="n">
+        <v>5</v>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>1.60</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>70.32</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>50.00</t>
+        </is>
+      </c>
+      <c r="M7" t="n">
+        <v>5</v>
+      </c>
+      <c r="N7" t="n">
+        <v>5</v>
+      </c>
+      <c r="O7" t="n">
+        <v>4</v>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>21.39</t>
+        </is>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>0.66</t>
+        </is>
+      </c>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>16.69</t>
+        </is>
+      </c>
+      <c r="S7" t="inlineStr">
+        <is>
+          <t>45.19</t>
+        </is>
+      </c>
+      <c r="T7" t="inlineStr">
+        <is>
+          <t>2022-Q1</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="6" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>001054</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>工银新金融股票</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>大盘成长</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>鄢耀</t>
+        </is>
+      </c>
+      <c r="F8" s="8" t="n">
+        <v>42082</v>
+      </c>
+      <c r="G8" s="8" t="n">
+        <v>42082</v>
+      </c>
+      <c r="H8" t="n">
+        <v>5</v>
+      </c>
+      <c r="I8" t="n">
+        <v>5</v>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>1.58</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>92.41</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>43.27</t>
+        </is>
+      </c>
+      <c r="M8" t="n">
+        <v>3</v>
+      </c>
+      <c r="N8" t="n">
+        <v>3</v>
+      </c>
+      <c r="O8" t="n">
+        <v>3</v>
+      </c>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>26.03</t>
+        </is>
+      </c>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>0.93</t>
+        </is>
+      </c>
+      <c r="R8" t="inlineStr">
+        <is>
+          <t>21.19</t>
+        </is>
+      </c>
+      <c r="S8" t="inlineStr">
+        <is>
+          <t>72.99</t>
+        </is>
+      </c>
+      <c r="T8" t="inlineStr">
+        <is>
+          <t>2022-Q1</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="6" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>450004</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>国富深化价值混合</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>大盘成长</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>刘晓</t>
+        </is>
+      </c>
+      <c r="F9" s="8" t="n">
+        <v>42784</v>
+      </c>
+      <c r="G9" s="8" t="n">
+        <v>39632</v>
+      </c>
+      <c r="H9" t="n">
+        <v>5</v>
+      </c>
+      <c r="I9" t="n">
+        <v>5</v>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>1.58</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>79.82</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>20.32</t>
+        </is>
+      </c>
+      <c r="M9" t="n">
+        <v>4</v>
+      </c>
+      <c r="N9" t="n">
+        <v>4</v>
+      </c>
+      <c r="O9" t="n">
+        <v>4</v>
+      </c>
+      <c r="P9" t="inlineStr">
+        <is>
+          <t>24.02</t>
+        </is>
+      </c>
+      <c r="Q9" t="inlineStr">
+        <is>
+          <t>0.80</t>
+        </is>
+      </c>
+      <c r="R9" t="inlineStr">
+        <is>
+          <t>19.28</t>
+        </is>
+      </c>
+      <c r="S9" t="inlineStr">
+        <is>
+          <t>36.11</t>
+        </is>
+      </c>
+      <c r="T9" t="inlineStr">
+        <is>
+          <t>2022-Q1</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="6" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>163807</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>中银优选混合</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>大盘成长</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>王伟</t>
+        </is>
+      </c>
+      <c r="F10" s="8" t="n">
+        <v>42152</v>
+      </c>
+      <c r="G10" s="8" t="n">
+        <v>39906</v>
+      </c>
+      <c r="H10" t="n">
+        <v>5</v>
+      </c>
+      <c r="I10" t="n">
+        <v>5</v>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>1.55</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>72.71</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>23.80</t>
+        </is>
+      </c>
+      <c r="M10" t="n">
+        <v>3</v>
+      </c>
+      <c r="N10" t="n">
+        <v>3</v>
+      </c>
+      <c r="O10" t="n">
+        <v>4</v>
+      </c>
+      <c r="P10" t="inlineStr">
+        <is>
+          <t>25.39</t>
+        </is>
+      </c>
+      <c r="Q10" t="inlineStr">
+        <is>
+          <t>0.64</t>
+        </is>
+      </c>
+      <c r="R10" t="inlineStr">
+        <is>
+          <t>19.66</t>
+        </is>
+      </c>
+      <c r="S10" t="inlineStr">
+        <is>
+          <t>30.26</t>
+        </is>
+      </c>
+      <c r="T10" t="inlineStr">
+        <is>
+          <t>2022-Q1</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="6" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>003298</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>嘉实物流产业股票A</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>大盘价值</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>肖觅</t>
+        </is>
+      </c>
+      <c r="F11" s="8" t="n">
+        <v>42733</v>
+      </c>
+      <c r="G11" s="8" t="n">
+        <v>42733</v>
+      </c>
+      <c r="H11" t="n">
+        <v>5</v>
+      </c>
+      <c r="I11" t="n">
+        <v>5</v>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>1.55</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>86.21</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>52.33</t>
+        </is>
+      </c>
+      <c r="M11" t="n">
+        <v>5</v>
+      </c>
+      <c r="N11" t="n">
+        <v>5</v>
+      </c>
+      <c r="O11" t="n">
+        <v>4</v>
+      </c>
+      <c r="P11" t="inlineStr">
+        <is>
+          <t>20.40</t>
+        </is>
+      </c>
+      <c r="Q11" t="inlineStr">
+        <is>
+          <t>0.68</t>
+        </is>
+      </c>
+      <c r="R11" t="inlineStr">
+        <is>
+          <t>14.51</t>
+        </is>
+      </c>
+      <c r="S11" t="inlineStr">
+        <is>
+          <t>9.55</t>
+        </is>
+      </c>
+      <c r="T11" t="inlineStr">
+        <is>
+          <t>2022-Q1</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="6" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>166301</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>华商新趋势优选灵活配置混合</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>大盘价值</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>周海栋</t>
+        </is>
+      </c>
+      <c r="F12" s="8" t="n">
+        <v>42138</v>
+      </c>
+      <c r="G12" s="8" t="n">
+        <v>42138</v>
+      </c>
+      <c r="H12" t="n">
+        <v>5</v>
+      </c>
+      <c r="I12" t="n">
+        <v>5</v>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>1.55</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>86.39</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>32.49</t>
+        </is>
+      </c>
+      <c r="M12" t="n">
+        <v>2</v>
+      </c>
+      <c r="N12" t="n">
+        <v>2</v>
+      </c>
+      <c r="O12" t="n">
+        <v>2</v>
+      </c>
+      <c r="P12" t="inlineStr"/>
+      <c r="Q12" t="inlineStr"/>
+      <c r="R12" t="inlineStr">
+        <is>
+          <t>23.84</t>
+        </is>
+      </c>
+      <c r="S12" t="inlineStr">
+        <is>
+          <t>26.96</t>
+        </is>
+      </c>
+      <c r="T12" t="inlineStr">
+        <is>
+          <t>2022-Q1</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="6" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>001445</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>华安国企改革主题灵活配置混合</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>大盘平衡</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>张亮</t>
+        </is>
+      </c>
+      <c r="F13" s="8" t="n">
+        <v>43404</v>
+      </c>
+      <c r="G13" s="8" t="n">
+        <v>42184</v>
+      </c>
+      <c r="H13" t="n">
+        <v>5</v>
+      </c>
+      <c r="I13" t="n">
+        <v>5</v>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>1.54</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>87.35</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>39.46</t>
+        </is>
+      </c>
+      <c r="M13" t="n">
+        <v>4</v>
+      </c>
+      <c r="N13" t="n">
+        <v>4</v>
+      </c>
+      <c r="O13" t="n">
+        <v>4</v>
+      </c>
+      <c r="P13" t="inlineStr">
+        <is>
+          <t>23.00</t>
+        </is>
+      </c>
+      <c r="Q13" t="inlineStr">
+        <is>
+          <t>0.70</t>
+        </is>
+      </c>
+      <c r="R13" t="inlineStr">
+        <is>
+          <t>18.59</t>
+        </is>
+      </c>
+      <c r="S13" t="inlineStr">
+        <is>
+          <t>47.50</t>
+        </is>
+      </c>
+      <c r="T13" t="inlineStr">
+        <is>
+          <t>2022-Q1</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="6" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>530006</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>建信核心精选混合</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>大盘平衡</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>王东杰</t>
+        </is>
+      </c>
+      <c r="F14" s="8" t="n">
+        <v>42975</v>
+      </c>
+      <c r="G14" s="8" t="n">
+        <v>39777</v>
+      </c>
+      <c r="H14" t="n">
+        <v>5</v>
+      </c>
+      <c r="I14" t="n">
+        <v>5</v>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>1.51</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>66.63</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>59.51</t>
+        </is>
+      </c>
+      <c r="M14" t="n">
+        <v>5</v>
+      </c>
+      <c r="N14" t="n">
+        <v>5</v>
+      </c>
+      <c r="O14" t="n">
+        <v>4</v>
+      </c>
+      <c r="P14" t="inlineStr">
+        <is>
+          <t>19.90</t>
+        </is>
+      </c>
+      <c r="Q14" t="inlineStr">
+        <is>
+          <t>0.72</t>
+        </is>
+      </c>
+      <c r="R14" t="inlineStr">
+        <is>
+          <t>16.98</t>
+        </is>
+      </c>
+      <c r="S14" t="inlineStr">
+        <is>
+          <t>4.34</t>
+        </is>
+      </c>
+      <c r="T14" t="inlineStr">
+        <is>
+          <t>2022-Q1</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="6" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>519918</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>华夏兴和混合</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>大盘价值</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>李彦</t>
+        </is>
+      </c>
+      <c r="F15" s="8" t="n">
+        <v>43994</v>
+      </c>
+      <c r="G15" s="8" t="n">
+        <v>41789</v>
+      </c>
+      <c r="H15" t="n">
+        <v>5</v>
+      </c>
+      <c r="I15" t="n">
+        <v>5</v>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>1.50</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>82.18</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>48.05</t>
+        </is>
+      </c>
+      <c r="M15" t="n">
+        <v>2</v>
+      </c>
+      <c r="N15" t="n">
+        <v>2</v>
+      </c>
+      <c r="O15" t="n">
+        <v>2</v>
+      </c>
+      <c r="P15" t="inlineStr">
+        <is>
+          <t>33.02</t>
+        </is>
+      </c>
+      <c r="Q15" t="inlineStr">
+        <is>
+          <t>0.55</t>
+        </is>
+      </c>
+      <c r="R15" t="inlineStr">
+        <is>
+          <t>24.98</t>
+        </is>
+      </c>
+      <c r="S15" t="inlineStr">
+        <is>
+          <t>53.07</t>
+        </is>
+      </c>
+      <c r="T15" t="inlineStr">
+        <is>
+          <t>2022-Q1</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="6" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>000547</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>建信健康民生混合</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>大盘成长</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>姜锋</t>
+        </is>
+      </c>
+      <c r="F16" s="8" t="n">
+        <v>41719</v>
+      </c>
+      <c r="G16" s="8" t="n">
+        <v>41719</v>
+      </c>
+      <c r="H16" t="n">
+        <v>5</v>
+      </c>
+      <c r="I16" t="n">
+        <v>5</v>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>1.49</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>82.38</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>37.18</t>
+        </is>
+      </c>
+      <c r="M16" t="n">
+        <v>3</v>
+      </c>
+      <c r="N16" t="n">
+        <v>3</v>
+      </c>
+      <c r="O16" t="n">
+        <v>3</v>
+      </c>
+      <c r="P16" t="inlineStr">
+        <is>
+          <t>25.27</t>
+        </is>
+      </c>
+      <c r="Q16" t="inlineStr">
+        <is>
+          <t>0.73</t>
+        </is>
+      </c>
+      <c r="R16" t="inlineStr">
+        <is>
+          <t>20.92</t>
+        </is>
+      </c>
+      <c r="S16" t="inlineStr">
+        <is>
+          <t>10.70</t>
+        </is>
+      </c>
+      <c r="T16" t="inlineStr">
+        <is>
+          <t>2022-Q1</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="6" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>121008</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>国投瑞银成长优选混合</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>大盘成长</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>桑俊</t>
+        </is>
+      </c>
+      <c r="F17" s="8" t="n">
+        <v>43106</v>
+      </c>
+      <c r="G17" s="8" t="n">
+        <v>39457</v>
+      </c>
+      <c r="H17" t="n">
+        <v>5</v>
+      </c>
+      <c r="I17" t="n">
+        <v>4</v>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>1.46</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>90.04</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>51.93</t>
+        </is>
+      </c>
+      <c r="M17" t="n">
+        <v>4</v>
+      </c>
+      <c r="N17" t="n">
+        <v>4</v>
+      </c>
+      <c r="O17" t="n">
+        <v>4</v>
+      </c>
+      <c r="P17" t="inlineStr">
+        <is>
+          <t>21.20</t>
+        </is>
+      </c>
+      <c r="Q17" t="inlineStr">
+        <is>
+          <t>0.74</t>
+        </is>
+      </c>
+      <c r="R17" t="inlineStr">
+        <is>
+          <t>18.55</t>
+        </is>
+      </c>
+      <c r="S17" t="inlineStr">
+        <is>
+          <t>5.76</t>
+        </is>
+      </c>
+      <c r="T17" t="inlineStr">
+        <is>
+          <t>2022-Q1</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="6" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>000592</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>建信改革红利股票</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>大盘成长</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>陶灿</t>
+        </is>
+      </c>
+      <c r="F18" s="8" t="n">
+        <v>41773</v>
+      </c>
+      <c r="G18" s="8" t="n">
+        <v>41773</v>
+      </c>
+      <c r="H18" t="n">
+        <v>5</v>
+      </c>
+      <c r="I18" t="n">
+        <v>5</v>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>1.45</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>91.05</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>36.37</t>
+        </is>
+      </c>
+      <c r="M18" t="n">
+        <v>2</v>
+      </c>
+      <c r="N18" t="n">
+        <v>2</v>
+      </c>
+      <c r="O18" t="n">
+        <v>2</v>
+      </c>
+      <c r="P18" t="inlineStr">
+        <is>
+          <t>29.27</t>
+        </is>
+      </c>
+      <c r="Q18" t="inlineStr">
+        <is>
+          <t>0.85</t>
+        </is>
+      </c>
+      <c r="R18" t="inlineStr">
+        <is>
+          <t>24.84</t>
+        </is>
+      </c>
+      <c r="S18" t="inlineStr">
+        <is>
+          <t>9.09</t>
+        </is>
+      </c>
+      <c r="T18" t="inlineStr">
+        <is>
+          <t>2022-Q1</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="6" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>003961</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>易方达瑞程灵活配置混合A</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>大盘成长</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>林森</t>
+        </is>
+      </c>
+      <c r="F19" s="8" t="n">
+        <v>42761</v>
+      </c>
+      <c r="G19" s="8" t="n">
+        <v>42719</v>
+      </c>
+      <c r="H19" t="n">
+        <v>5</v>
+      </c>
+      <c r="I19" t="n">
+        <v>5</v>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>1.44</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>91.05</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>45.28</t>
+        </is>
+      </c>
+      <c r="M19" t="n">
+        <v>3</v>
+      </c>
+      <c r="N19" t="n">
+        <v>2</v>
+      </c>
+      <c r="O19" t="n">
+        <v>2</v>
+      </c>
+      <c r="P19" t="inlineStr">
+        <is>
+          <t>27.54</t>
+        </is>
+      </c>
+      <c r="Q19" t="inlineStr">
+        <is>
+          <t>0.92</t>
+        </is>
+      </c>
+      <c r="R19" t="inlineStr">
+        <is>
+          <t>24.22</t>
+        </is>
+      </c>
+      <c r="S19" t="inlineStr">
+        <is>
+          <t>34.99</t>
+        </is>
+      </c>
+      <c r="T19" t="inlineStr">
+        <is>
+          <t>2022-Q1</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="6" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>163810</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>中银价值精选灵活配置混合</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>大盘平衡</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>王睿</t>
+        </is>
+      </c>
+      <c r="F20" s="8" t="n">
+        <v>43726</v>
+      </c>
+      <c r="G20" s="8" t="n">
+        <v>40415</v>
+      </c>
+      <c r="H20" t="n">
+        <v>5</v>
+      </c>
+      <c r="I20" t="n">
+        <v>4</v>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>1.44</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>76.15</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>31.98</t>
+        </is>
+      </c>
+      <c r="M20" t="n">
+        <v>3</v>
+      </c>
+      <c r="N20" t="n">
+        <v>3</v>
+      </c>
+      <c r="O20" t="n">
+        <v>3</v>
+      </c>
+      <c r="P20" t="inlineStr">
+        <is>
+          <t>19.90</t>
+        </is>
+      </c>
+      <c r="Q20" t="inlineStr">
+        <is>
+          <t>1.56</t>
+        </is>
+      </c>
+      <c r="R20" t="inlineStr">
+        <is>
+          <t>17.35</t>
+        </is>
+      </c>
+      <c r="S20" t="inlineStr">
+        <is>
+          <t>1.90</t>
+        </is>
+      </c>
+      <c r="T20" t="inlineStr">
+        <is>
+          <t>2022-Q1</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="6" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>001959</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>华商乐享互联灵活配置混合</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>大盘平衡</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>周海栋</t>
+        </is>
+      </c>
+      <c r="F21" s="8" t="n">
+        <v>43430</v>
+      </c>
+      <c r="G21" s="8" t="n">
+        <v>42356</v>
+      </c>
+      <c r="H21" t="n">
+        <v>5</v>
+      </c>
+      <c r="I21" t="n">
+        <v>3</v>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>1.43</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>88.84</t>
+        </is>
+      </c>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>38.52</t>
+        </is>
+      </c>
+      <c r="M21" t="n">
+        <v>3</v>
+      </c>
+      <c r="N21" t="n">
+        <v>2</v>
+      </c>
+      <c r="O21" t="n">
+        <v>2</v>
+      </c>
+      <c r="P21" t="inlineStr">
+        <is>
+          <t>30.29</t>
+        </is>
+      </c>
+      <c r="Q21" t="inlineStr">
+        <is>
+          <t>0.54</t>
+        </is>
+      </c>
+      <c r="R21" t="inlineStr">
+        <is>
+          <t>24.13</t>
+        </is>
+      </c>
+      <c r="S21" t="inlineStr">
+        <is>
+          <t>3.74</t>
+        </is>
+      </c>
+      <c r="T21" t="inlineStr">
+        <is>
+          <t>2022-Q1</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="6" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>002910</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>易方达供给改革灵活配置混合</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>中盘平衡</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>杨宗昌</t>
+        </is>
+      </c>
+      <c r="F22" s="8" t="n">
+        <v>43578</v>
+      </c>
+      <c r="G22" s="8" t="n">
+        <v>42760</v>
+      </c>
+      <c r="H22" t="n">
+        <v>5</v>
+      </c>
+      <c r="I22" t="n">
+        <v>4</v>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>1.43</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>87.54</t>
+        </is>
+      </c>
+      <c r="L22" t="inlineStr">
+        <is>
+          <t>56.47</t>
+        </is>
+      </c>
+      <c r="M22" t="n">
+        <v>2</v>
+      </c>
+      <c r="N22" t="n">
+        <v>2</v>
+      </c>
+      <c r="O22" t="n">
+        <v>3</v>
+      </c>
+      <c r="P22" t="inlineStr">
+        <is>
+          <t>29.22</t>
+        </is>
+      </c>
+      <c r="Q22" t="inlineStr">
+        <is>
+          <t>1.17</t>
+        </is>
+      </c>
+      <c r="R22" t="inlineStr">
+        <is>
+          <t>24.21</t>
+        </is>
+      </c>
+      <c r="S22" t="inlineStr">
+        <is>
+          <t>49.29</t>
+        </is>
+      </c>
+      <c r="T22" t="inlineStr">
+        <is>
+          <t>2022-Q1</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="6" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>519126</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>浦银安盛新经济结构灵活配置混合</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>大盘成长</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>蒋佳良</t>
+        </is>
+      </c>
+      <c r="F23" s="8" t="n">
+        <v>43405</v>
+      </c>
+      <c r="G23" s="8" t="n">
+        <v>41779</v>
+      </c>
+      <c r="H23" t="n">
+        <v>5</v>
+      </c>
+      <c r="I23" t="n">
+        <v>4</v>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>1.43</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>87.78</t>
+        </is>
+      </c>
+      <c r="L23" t="inlineStr">
+        <is>
+          <t>42.42</t>
+        </is>
+      </c>
+      <c r="M23" t="n">
+        <v>2</v>
+      </c>
+      <c r="N23" t="n">
+        <v>2</v>
+      </c>
+      <c r="O23" t="n">
+        <v>2</v>
+      </c>
+      <c r="P23" t="inlineStr">
+        <is>
+          <t>27.07</t>
+        </is>
+      </c>
+      <c r="Q23" t="inlineStr">
+        <is>
+          <t>0.87</t>
+        </is>
+      </c>
+      <c r="R23" t="inlineStr">
+        <is>
+          <t>23.78</t>
+        </is>
+      </c>
+      <c r="S23" t="inlineStr">
+        <is>
+          <t>40.94</t>
+        </is>
+      </c>
+      <c r="T23" t="inlineStr">
+        <is>
+          <t>2022-Q1</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="6" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>001864</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>中海魅力长三角灵活配置混合</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>大盘成长</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>陈星</t>
+        </is>
+      </c>
+      <c r="F24" s="8" t="n">
+        <v>44023</v>
+      </c>
+      <c r="G24" s="8" t="n">
+        <v>42459</v>
+      </c>
+      <c r="H24" t="n">
+        <v>5</v>
+      </c>
+      <c r="I24" t="n">
+        <v>5</v>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>1.42</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>74.64</t>
+        </is>
+      </c>
+      <c r="L24" t="inlineStr">
+        <is>
+          <t>34.53</t>
+        </is>
+      </c>
+      <c r="M24" t="n">
+        <v>3</v>
+      </c>
+      <c r="N24" t="n">
+        <v>2</v>
+      </c>
+      <c r="O24" t="n">
+        <v>2</v>
+      </c>
+      <c r="P24" t="inlineStr">
+        <is>
+          <t>23.81</t>
+        </is>
+      </c>
+      <c r="Q24" t="inlineStr">
+        <is>
+          <t>1.43</t>
+        </is>
+      </c>
+      <c r="R24" t="inlineStr">
+        <is>
+          <t>20.01</t>
+        </is>
+      </c>
+      <c r="S24" t="inlineStr">
+        <is>
+          <t>0.22</t>
+        </is>
+      </c>
+      <c r="T24" t="inlineStr">
+        <is>
+          <t>2022-Q1</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="6" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>001457</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>华商新常态灵活配置混合</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>大盘成长</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>吴昊</t>
+        </is>
+      </c>
+      <c r="F25" s="8" t="n">
+        <v>43293</v>
+      </c>
+      <c r="G25" s="8" t="n">
+        <v>42184</v>
+      </c>
+      <c r="H25" t="n">
+        <v>5</v>
+      </c>
+      <c r="I25" t="n">
+        <v>3</v>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>1.42</t>
+        </is>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>83.98</t>
+        </is>
+      </c>
+      <c r="L25" t="inlineStr">
+        <is>
+          <t>35.72</t>
+        </is>
+      </c>
+      <c r="M25" t="n">
+        <v>3</v>
+      </c>
+      <c r="N25" t="n">
+        <v>3</v>
+      </c>
+      <c r="O25" t="n">
+        <v>3</v>
+      </c>
+      <c r="P25" t="inlineStr">
+        <is>
+          <t>21.95</t>
+        </is>
+      </c>
+      <c r="Q25" t="inlineStr">
+        <is>
+          <t>0.77</t>
+        </is>
+      </c>
+      <c r="R25" t="inlineStr">
+        <is>
+          <t>19.86</t>
+        </is>
+      </c>
+      <c r="S25" t="inlineStr">
+        <is>
+          <t>2.32</t>
+        </is>
+      </c>
+      <c r="T25" t="inlineStr">
+        <is>
+          <t>2022-Q1</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="6" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>000165</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>国投瑞银策略精选混合</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>大盘成长</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>吉莉</t>
+        </is>
+      </c>
+      <c r="F26" s="8" t="n">
+        <v>43106</v>
+      </c>
+      <c r="G26" s="8" t="n">
+        <v>41544</v>
+      </c>
+      <c r="H26" t="n">
+        <v>5</v>
+      </c>
+      <c r="I26" t="n">
+        <v>5</v>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>1.42</t>
+        </is>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>70.38</t>
+        </is>
+      </c>
+      <c r="L26" t="inlineStr">
+        <is>
+          <t>22.07</t>
+        </is>
+      </c>
+      <c r="M26" t="n">
+        <v>3</v>
+      </c>
+      <c r="N26" t="n">
+        <v>3</v>
+      </c>
+      <c r="O26" t="n">
+        <v>3</v>
+      </c>
+      <c r="P26" t="inlineStr">
+        <is>
+          <t>19.91</t>
+        </is>
+      </c>
+      <c r="Q26" t="inlineStr">
+        <is>
+          <t>1.14</t>
+        </is>
+      </c>
+      <c r="R26" t="inlineStr">
+        <is>
+          <t>16.68</t>
+        </is>
+      </c>
+      <c r="S26" t="inlineStr">
+        <is>
+          <t>3.38</t>
+        </is>
+      </c>
+      <c r="T26" t="inlineStr">
+        <is>
+          <t>2022-Q1</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="6" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>001366</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>金鹰产业整合灵活配置混合</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>大盘成长</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>杨晓斌</t>
+        </is>
+      </c>
+      <c r="F27" s="8" t="n">
+        <v>43538</v>
+      </c>
+      <c r="G27" s="8" t="n">
+        <v>42171</v>
+      </c>
+      <c r="H27" t="n">
+        <v>5</v>
+      </c>
+      <c r="I27" t="n">
+        <v>4</v>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>1.40</t>
+        </is>
+      </c>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>91.56</t>
+        </is>
+      </c>
+      <c r="L27" t="inlineStr">
+        <is>
+          <t>34.44</t>
+        </is>
+      </c>
+      <c r="M27" t="n">
+        <v>3</v>
+      </c>
+      <c r="N27" t="n">
+        <v>3</v>
+      </c>
+      <c r="O27" t="n">
+        <v>3</v>
+      </c>
+      <c r="P27" t="inlineStr">
+        <is>
+          <t>22.82</t>
+        </is>
+      </c>
+      <c r="Q27" t="inlineStr">
+        <is>
+          <t>0.85</t>
+        </is>
+      </c>
+      <c r="R27" t="inlineStr">
+        <is>
+          <t>21.13</t>
+        </is>
+      </c>
+      <c r="S27" t="inlineStr">
+        <is>
+          <t>5.27</t>
+        </is>
+      </c>
+      <c r="T27" t="inlineStr">
+        <is>
+          <t>2022-Q1</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="6" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>163822</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>中银主题策略混合</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>大盘成长</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>黄珺</t>
+        </is>
+      </c>
+      <c r="F28" s="8" t="n">
+        <v>43537</v>
+      </c>
+      <c r="G28" s="8" t="n">
+        <v>41115</v>
+      </c>
+      <c r="H28" t="n">
+        <v>5</v>
+      </c>
+      <c r="I28" t="n">
+        <v>3</v>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>1.39</t>
+        </is>
+      </c>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>84.73</t>
+        </is>
+      </c>
+      <c r="L28" t="inlineStr">
+        <is>
+          <t>36.78</t>
+        </is>
+      </c>
+      <c r="M28" t="n">
+        <v>3</v>
+      </c>
+      <c r="N28" t="n">
+        <v>3</v>
+      </c>
+      <c r="O28" t="n">
+        <v>3</v>
+      </c>
+      <c r="P28" t="inlineStr">
+        <is>
+          <t>24.50</t>
+        </is>
+      </c>
+      <c r="Q28" t="inlineStr">
+        <is>
+          <t>0.67</t>
+        </is>
+      </c>
+      <c r="R28" t="inlineStr">
+        <is>
+          <t>21.54</t>
+        </is>
+      </c>
+      <c r="S28" t="inlineStr">
+        <is>
+          <t>7.89</t>
+        </is>
+      </c>
+      <c r="T28" t="inlineStr">
+        <is>
+          <t>2022-Q1</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="6" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>000390</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>华商优势行业混合</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>大盘价值</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>周海栋</t>
+        </is>
+      </c>
+      <c r="F29" s="8" t="n">
+        <v>42587</v>
+      </c>
+      <c r="G29" s="8" t="n">
+        <v>41619</v>
+      </c>
+      <c r="H29" t="n">
+        <v>5</v>
+      </c>
+      <c r="I29" t="n">
+        <v>5</v>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>1.38</t>
+        </is>
+      </c>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>88.06</t>
+        </is>
+      </c>
+      <c r="L29" t="inlineStr">
+        <is>
+          <t>36.18</t>
+        </is>
+      </c>
+      <c r="M29" t="n">
+        <v>3</v>
+      </c>
+      <c r="N29" t="n">
+        <v>3</v>
+      </c>
+      <c r="O29" t="n">
+        <v>3</v>
+      </c>
+      <c r="P29" t="inlineStr">
+        <is>
+          <t>25.95</t>
+        </is>
+      </c>
+      <c r="Q29" t="inlineStr">
+        <is>
+          <t>0.38</t>
+        </is>
+      </c>
+      <c r="R29" t="inlineStr">
+        <is>
+          <t>20.95</t>
+        </is>
+      </c>
+      <c r="S29" t="inlineStr">
+        <is>
+          <t>19.61</t>
+        </is>
+      </c>
+      <c r="T29" t="inlineStr">
+        <is>
+          <t>2022-Q1</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="6" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>002669</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>华商万众创新灵活配置混合</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>大盘成长</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>梁皓</t>
+        </is>
+      </c>
+      <c r="F30" s="8" t="n">
+        <v>43039</v>
+      </c>
+      <c r="G30" s="8" t="n">
+        <v>42549</v>
+      </c>
+      <c r="H30" t="n">
+        <v>5</v>
+      </c>
+      <c r="I30" t="n">
+        <v>4</v>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>1.37</t>
+        </is>
+      </c>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>83.72</t>
+        </is>
+      </c>
+      <c r="L30" t="inlineStr">
+        <is>
+          <t>45.84</t>
+        </is>
+      </c>
+      <c r="M30" t="n">
+        <v>2</v>
+      </c>
+      <c r="N30" t="n">
+        <v>2</v>
+      </c>
+      <c r="O30" t="n">
+        <v>2</v>
+      </c>
+      <c r="P30" t="inlineStr">
+        <is>
+          <t>29.09</t>
+        </is>
+      </c>
+      <c r="Q30" t="inlineStr">
+        <is>
+          <t>0.84</t>
+        </is>
+      </c>
+      <c r="R30" t="inlineStr">
+        <is>
+          <t>26.11</t>
+        </is>
+      </c>
+      <c r="S30" t="inlineStr">
+        <is>
+          <t>18.97</t>
+        </is>
+      </c>
+      <c r="T30" t="inlineStr">
+        <is>
+          <t>2022-Q1</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="6" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>160421</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>华安智增精选灵活配置混合（LOF）</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>大盘成长</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>王春</t>
+        </is>
+      </c>
+      <c r="F31" s="8" t="n">
+        <v>43157</v>
+      </c>
+      <c r="G31" s="8" t="n">
+        <v>42626</v>
+      </c>
+      <c r="H31" t="n">
+        <v>5</v>
+      </c>
+      <c r="I31" t="n">
+        <v>5</v>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>1.36</t>
+        </is>
+      </c>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>84.67</t>
+        </is>
+      </c>
+      <c r="L31" t="inlineStr">
+        <is>
+          <t>53.16</t>
+        </is>
+      </c>
+      <c r="M31" t="n">
+        <v>2</v>
+      </c>
+      <c r="N31" t="n">
+        <v>2</v>
+      </c>
+      <c r="O31" t="n">
+        <v>2</v>
+      </c>
+      <c r="P31" t="inlineStr">
+        <is>
+          <t>29.99</t>
+        </is>
+      </c>
+      <c r="Q31" t="inlineStr">
+        <is>
+          <t>0.52</t>
+        </is>
+      </c>
+      <c r="R31" t="inlineStr">
+        <is>
+          <t>25.08</t>
+        </is>
+      </c>
+      <c r="S31" t="inlineStr">
+        <is>
+          <t>2.11</t>
+        </is>
+      </c>
+      <c r="T31" t="inlineStr">
+        <is>
+          <t>2022-Q1</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="6" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>000259</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>农银区间收益混合</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>大盘成长</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>魏刚</t>
+        </is>
+      </c>
+      <c r="F32" s="8" t="n">
+        <v>43861</v>
+      </c>
+      <c r="G32" s="8" t="n">
+        <v>41507</v>
+      </c>
+      <c r="H32" t="n">
+        <v>5</v>
+      </c>
+      <c r="I32" t="n">
+        <v>5</v>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>1.36</t>
+        </is>
+      </c>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>65.11</t>
+        </is>
+      </c>
+      <c r="L32" t="inlineStr">
+        <is>
+          <t>22.56</t>
+        </is>
+      </c>
+      <c r="M32" t="n">
+        <v>3</v>
+      </c>
+      <c r="N32" t="n">
+        <v>3</v>
+      </c>
+      <c r="O32" t="n">
+        <v>3</v>
+      </c>
+      <c r="P32" t="inlineStr">
+        <is>
+          <t>18.73</t>
+        </is>
+      </c>
+      <c r="Q32" t="inlineStr">
+        <is>
+          <t>1.35</t>
+        </is>
+      </c>
+      <c r="R32" t="inlineStr">
+        <is>
+          <t>16.96</t>
+        </is>
+      </c>
+      <c r="S32" t="inlineStr">
+        <is>
+          <t>4.01</t>
+        </is>
+      </c>
+      <c r="T32" t="inlineStr">
+        <is>
+          <t>2022-Q1</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="6" t="n">
+        <v>31</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>400032</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>东方主题精选混合</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>中盘成长</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>蒋茜</t>
+        </is>
+      </c>
+      <c r="F33" s="8" t="n">
+        <v>43467</v>
+      </c>
+      <c r="G33" s="8" t="n">
+        <v>42086</v>
+      </c>
+      <c r="H33" t="n">
+        <v>5</v>
+      </c>
+      <c r="I33" t="n">
+        <v>3</v>
+      </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>1.35</t>
+        </is>
+      </c>
+      <c r="K33" t="inlineStr">
+        <is>
+          <t>85.31</t>
+        </is>
+      </c>
+      <c r="L33" t="inlineStr">
+        <is>
+          <t>36.64</t>
+        </is>
+      </c>
+      <c r="M33" t="n">
+        <v>2</v>
+      </c>
+      <c r="N33" t="n">
+        <v>2</v>
+      </c>
+      <c r="O33" t="n">
+        <v>2</v>
+      </c>
+      <c r="P33" t="inlineStr">
+        <is>
+          <t>29.01</t>
+        </is>
+      </c>
+      <c r="Q33" t="inlineStr">
+        <is>
+          <t>0.90</t>
+        </is>
+      </c>
+      <c r="R33" t="inlineStr">
+        <is>
+          <t>26.76</t>
+        </is>
+      </c>
+      <c r="S33" t="inlineStr">
+        <is>
+          <t>29.31</t>
+        </is>
+      </c>
+      <c r="T33" t="inlineStr">
+        <is>
+          <t>2022-Q1</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="6" t="n">
+        <v>32</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>000756</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>建信潜力新蓝筹股票</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>中盘成长</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>周智硕</t>
+        </is>
+      </c>
+      <c r="F34" s="8" t="n">
+        <v>44092</v>
+      </c>
+      <c r="G34" s="8" t="n">
+        <v>41892</v>
+      </c>
+      <c r="H34" t="n">
+        <v>5</v>
+      </c>
+      <c r="I34" t="n">
+        <v>4</v>
+      </c>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>1.33</t>
+        </is>
+      </c>
+      <c r="K34" t="inlineStr">
+        <is>
+          <t>84.61</t>
+        </is>
+      </c>
+      <c r="L34" t="inlineStr">
+        <is>
+          <t>46.80</t>
+        </is>
+      </c>
+      <c r="M34" t="n">
+        <v>2</v>
+      </c>
+      <c r="N34" t="n">
+        <v>2</v>
+      </c>
+      <c r="O34" t="n">
+        <v>2</v>
+      </c>
+      <c r="P34" t="inlineStr">
+        <is>
+          <t>24.54</t>
+        </is>
+      </c>
+      <c r="Q34" t="inlineStr">
+        <is>
+          <t>0.76</t>
+        </is>
+      </c>
+      <c r="R34" t="inlineStr">
+        <is>
+          <t>22.97</t>
+        </is>
+      </c>
+      <c r="S34" t="inlineStr">
+        <is>
+          <t>10.47</t>
+        </is>
+      </c>
+      <c r="T34" t="inlineStr">
+        <is>
+          <t>2022-Q1</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="6" t="n">
+        <v>33</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>003152</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>华富天鑫灵活配置混合A</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>大盘成长</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>陈启明</t>
+        </is>
+      </c>
+      <c r="F35" s="8" t="n">
+        <v>43490</v>
+      </c>
+      <c r="G35" s="8" t="n">
+        <v>42733</v>
+      </c>
+      <c r="H35" t="n">
+        <v>5</v>
+      </c>
+      <c r="I35" t="n">
+        <v>3</v>
+      </c>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t>1.33</t>
+        </is>
+      </c>
+      <c r="K35" t="inlineStr">
+        <is>
+          <t>93.75</t>
+        </is>
+      </c>
+      <c r="L35" t="inlineStr">
+        <is>
+          <t>57.41</t>
+        </is>
+      </c>
+      <c r="M35" t="n">
+        <v>2</v>
+      </c>
+      <c r="N35" t="n">
+        <v>2</v>
+      </c>
+      <c r="O35" t="n">
+        <v>3</v>
+      </c>
+      <c r="P35" t="inlineStr">
+        <is>
+          <t>22.66</t>
+        </is>
+      </c>
+      <c r="Q35" t="inlineStr">
+        <is>
+          <t>1.30</t>
+        </is>
+      </c>
+      <c r="R35" t="inlineStr">
+        <is>
+          <t>20.23</t>
+        </is>
+      </c>
+      <c r="S35" t="inlineStr">
+        <is>
+          <t>1.59</t>
+        </is>
+      </c>
+      <c r="T35" t="inlineStr">
+        <is>
+          <t>2022-Q1</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="6" t="n">
+        <v>34</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>001359</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>国联安添鑫灵活配置混合A</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>大盘平衡</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>薛琳</t>
+        </is>
+      </c>
+      <c r="F36" s="8" t="n">
+        <v>42678</v>
+      </c>
+      <c r="G36" s="8" t="n">
+        <v>42157</v>
+      </c>
+      <c r="H36" t="n">
+        <v>5</v>
+      </c>
+      <c r="I36" t="n">
+        <v>4</v>
+      </c>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t>1.33</t>
+        </is>
+      </c>
+      <c r="K36" t="inlineStr">
+        <is>
+          <t>77.94</t>
+        </is>
+      </c>
+      <c r="L36" t="inlineStr">
+        <is>
+          <t>38.93</t>
+        </is>
+      </c>
+      <c r="M36" t="n">
+        <v>3</v>
+      </c>
+      <c r="N36" t="n">
+        <v>3</v>
+      </c>
+      <c r="O36" t="n">
+        <v>3</v>
+      </c>
+      <c r="P36" t="inlineStr">
+        <is>
+          <t>18.06</t>
+        </is>
+      </c>
+      <c r="Q36" t="inlineStr">
+        <is>
+          <t>1.65</t>
+        </is>
+      </c>
+      <c r="R36" t="inlineStr">
+        <is>
+          <t>17.59</t>
+        </is>
+      </c>
+      <c r="S36" t="inlineStr">
+        <is>
+          <t>0.46</t>
+        </is>
+      </c>
+      <c r="T36" t="inlineStr">
+        <is>
+          <t>2022-Q1</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="6" t="n">
+        <v>35</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>217013</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>招商中小盘精选混合</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>大盘成长</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>韩冰</t>
+        </is>
+      </c>
+      <c r="F37" s="8" t="n">
+        <v>42129</v>
+      </c>
+      <c r="G37" s="8" t="n">
+        <v>40172</v>
+      </c>
+      <c r="H37" t="n">
+        <v>5</v>
+      </c>
+      <c r="I37" t="n">
+        <v>5</v>
+      </c>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t>1.32</t>
+        </is>
+      </c>
+      <c r="K37" t="inlineStr">
+        <is>
+          <t>83.36</t>
+        </is>
+      </c>
+      <c r="L37" t="inlineStr">
+        <is>
+          <t>49.52</t>
+        </is>
+      </c>
+      <c r="M37" t="n">
+        <v>3</v>
+      </c>
+      <c r="N37" t="n">
+        <v>3</v>
+      </c>
+      <c r="O37" t="n">
+        <v>3</v>
+      </c>
+      <c r="P37" t="inlineStr">
+        <is>
+          <t>22.41</t>
+        </is>
+      </c>
+      <c r="Q37" t="inlineStr">
+        <is>
+          <t>0.94</t>
+        </is>
+      </c>
+      <c r="R37" t="inlineStr">
+        <is>
+          <t>22.62</t>
+        </is>
+      </c>
+      <c r="S37" t="inlineStr">
+        <is>
+          <t>2.53</t>
+        </is>
+      </c>
+      <c r="T37" t="inlineStr">
+        <is>
+          <t>2022-Q1</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="6" t="n">
+        <v>36</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>519756</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>交银施罗德国企改革灵活配置混合</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>大盘价值</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>沈楠</t>
+        </is>
+      </c>
+      <c r="F38" s="8" t="n">
+        <v>42165</v>
+      </c>
+      <c r="G38" s="8" t="n">
+        <v>42165</v>
+      </c>
+      <c r="H38" t="n">
+        <v>5</v>
+      </c>
+      <c r="I38" t="n">
+        <v>4</v>
+      </c>
+      <c r="J38" t="inlineStr">
+        <is>
+          <t>1.31</t>
+        </is>
+      </c>
+      <c r="K38" t="inlineStr">
+        <is>
+          <t>87.70</t>
+        </is>
+      </c>
+      <c r="L38" t="inlineStr">
+        <is>
+          <t>34.94</t>
+        </is>
+      </c>
+      <c r="M38" t="n">
+        <v>3</v>
+      </c>
+      <c r="N38" t="n">
+        <v>3</v>
+      </c>
+      <c r="O38" t="n">
+        <v>3</v>
+      </c>
+      <c r="P38" t="inlineStr">
+        <is>
+          <t>19.12</t>
+        </is>
+      </c>
+      <c r="Q38" t="inlineStr">
+        <is>
+          <t>0.87</t>
+        </is>
+      </c>
+      <c r="R38" t="inlineStr">
+        <is>
+          <t>16.71</t>
+        </is>
+      </c>
+      <c r="S38" t="inlineStr">
+        <is>
+          <t>5.69</t>
+        </is>
+      </c>
+      <c r="T38" t="inlineStr">
+        <is>
+          <t>2022-Q1</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="6" t="n">
+        <v>37</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>200015</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>长城优化升级混合</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>大盘成长</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>周诗博</t>
+        </is>
+      </c>
+      <c r="F39" s="8" t="n">
+        <v>44200</v>
+      </c>
+      <c r="G39" s="8" t="n">
+        <v>41019</v>
+      </c>
+      <c r="H39" t="n">
+        <v>5</v>
+      </c>
+      <c r="I39" t="n">
+        <v>5</v>
+      </c>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t>1.30</t>
+        </is>
+      </c>
+      <c r="K39" t="inlineStr">
+        <is>
+          <t>85.83</t>
+        </is>
+      </c>
+      <c r="L39" t="inlineStr">
+        <is>
+          <t>48.11</t>
+        </is>
+      </c>
+      <c r="M39" t="n">
+        <v>2</v>
+      </c>
+      <c r="N39" t="n">
+        <v>2</v>
+      </c>
+      <c r="O39" t="n">
+        <v>2</v>
+      </c>
+      <c r="P39" t="inlineStr">
+        <is>
+          <t>28.40</t>
+        </is>
+      </c>
+      <c r="Q39" t="inlineStr">
+        <is>
+          <t>0.75</t>
+        </is>
+      </c>
+      <c r="R39" t="inlineStr">
+        <is>
+          <t>26.35</t>
+        </is>
+      </c>
+      <c r="S39" t="inlineStr">
+        <is>
+          <t>18.17</t>
+        </is>
+      </c>
+      <c r="T39" t="inlineStr">
+        <is>
+          <t>2022-Q1</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="6" t="n">
+        <v>38</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>160624</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>鹏华消费领先混合</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>大盘成长</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>孟昊</t>
+        </is>
+      </c>
+      <c r="F40" s="8" t="n">
+        <v>43421</v>
+      </c>
+      <c r="G40" s="8" t="n">
+        <v>41631</v>
+      </c>
+      <c r="H40" t="n">
+        <v>5</v>
+      </c>
+      <c r="I40" t="n">
+        <v>5</v>
+      </c>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t>1.30</t>
+        </is>
+      </c>
+      <c r="K40" t="inlineStr">
+        <is>
+          <t>80.12</t>
+        </is>
+      </c>
+      <c r="L40" t="inlineStr">
+        <is>
+          <t>48.60</t>
+        </is>
+      </c>
+      <c r="M40" t="n">
+        <v>3</v>
+      </c>
+      <c r="N40" t="n">
+        <v>3</v>
+      </c>
+      <c r="O40" t="n">
+        <v>3</v>
+      </c>
+      <c r="P40" t="inlineStr">
+        <is>
+          <t>22.20</t>
+        </is>
+      </c>
+      <c r="Q40" t="inlineStr">
+        <is>
+          <t>0.87</t>
+        </is>
+      </c>
+      <c r="R40" t="inlineStr">
+        <is>
+          <t>22.44</t>
+        </is>
+      </c>
+      <c r="S40" t="inlineStr">
+        <is>
+          <t>5.83</t>
+        </is>
+      </c>
+      <c r="T40" t="inlineStr">
+        <is>
+          <t>2022-Q1</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="6" t="n">
+        <v>39</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>002846</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>泓德泓华灵活配置混合</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>大盘成长</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>秦毅</t>
+        </is>
+      </c>
+      <c r="F41" s="8" t="n">
+        <v>43461</v>
+      </c>
+      <c r="G41" s="8" t="n">
+        <v>42705</v>
+      </c>
+      <c r="H41" t="n">
+        <v>5</v>
+      </c>
+      <c r="I41" t="n">
+        <v>5</v>
+      </c>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t>1.30</t>
+        </is>
+      </c>
+      <c r="K41" t="inlineStr">
+        <is>
+          <t>93.24</t>
+        </is>
+      </c>
+      <c r="L41" t="inlineStr">
+        <is>
+          <t>47.66</t>
+        </is>
+      </c>
+      <c r="M41" t="n">
+        <v>2</v>
+      </c>
+      <c r="N41" t="n">
+        <v>3</v>
+      </c>
+      <c r="O41" t="n">
+        <v>3</v>
+      </c>
+      <c r="P41" t="inlineStr">
+        <is>
+          <t>21.42</t>
+        </is>
+      </c>
+      <c r="Q41" t="inlineStr">
+        <is>
+          <t>1.04</t>
+        </is>
+      </c>
+      <c r="R41" t="inlineStr">
+        <is>
+          <t>22.95</t>
+        </is>
+      </c>
+      <c r="S41" t="inlineStr">
+        <is>
+          <t>7.01</t>
+        </is>
+      </c>
+      <c r="T41" t="inlineStr">
+        <is>
+          <t>2022-Q1</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="6" t="n">
+        <v>40</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>530001</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>建信恒久价值混合</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>大盘成长</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>陶灿</t>
+        </is>
+      </c>
+      <c r="F42" s="8" t="n">
+        <v>42816</v>
+      </c>
+      <c r="G42" s="8" t="n">
+        <v>38687</v>
+      </c>
+      <c r="H42" t="n">
+        <v>5</v>
+      </c>
+      <c r="I42" t="n">
+        <v>4</v>
+      </c>
+      <c r="J42" t="inlineStr">
+        <is>
+          <t>1.29</t>
+        </is>
+      </c>
+      <c r="K42" t="inlineStr">
+        <is>
+          <t>91.57</t>
+        </is>
+      </c>
+      <c r="L42" t="inlineStr">
+        <is>
+          <t>40.39</t>
+        </is>
+      </c>
+      <c r="M42" t="n">
+        <v>2</v>
+      </c>
+      <c r="N42" t="n">
+        <v>2</v>
+      </c>
+      <c r="O42" t="n">
+        <v>2</v>
+      </c>
+      <c r="P42" t="inlineStr">
+        <is>
+          <t>25.66</t>
+        </is>
+      </c>
+      <c r="Q42" t="inlineStr">
+        <is>
+          <t>0.87</t>
+        </is>
+      </c>
+      <c r="R42" t="inlineStr">
+        <is>
+          <t>25.27</t>
+        </is>
+      </c>
+      <c r="S42" t="inlineStr">
+        <is>
+          <t>11.95</t>
+        </is>
+      </c>
+      <c r="T42" t="inlineStr">
+        <is>
+          <t>2022-Q1</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="6" t="n">
+        <v>41</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>210003</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>金鹰行业优势混合</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>大盘成长</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>倪超</t>
+        </is>
+      </c>
+      <c r="F43" s="8" t="n">
+        <v>42166</v>
+      </c>
+      <c r="G43" s="8" t="n">
+        <v>39995</v>
+      </c>
+      <c r="H43" t="n">
+        <v>5</v>
+      </c>
+      <c r="I43" t="n">
+        <v>5</v>
+      </c>
+      <c r="J43" t="inlineStr">
+        <is>
+          <t>1.28</t>
+        </is>
+      </c>
+      <c r="K43" t="inlineStr">
+        <is>
+          <t>88.02</t>
+        </is>
+      </c>
+      <c r="L43" t="inlineStr">
+        <is>
+          <t>44.86</t>
+        </is>
+      </c>
+      <c r="M43" t="n">
+        <v>2</v>
+      </c>
+      <c r="N43" t="n">
+        <v>2</v>
+      </c>
+      <c r="O43" t="n">
+        <v>2</v>
+      </c>
+      <c r="P43" t="inlineStr">
+        <is>
+          <t>27.53</t>
+        </is>
+      </c>
+      <c r="Q43" t="inlineStr">
+        <is>
+          <t>0.63</t>
+        </is>
+      </c>
+      <c r="R43" t="inlineStr">
+        <is>
+          <t>25.45</t>
+        </is>
+      </c>
+      <c r="S43" t="inlineStr">
+        <is>
+          <t>6.62</t>
+        </is>
+      </c>
+      <c r="T43" t="inlineStr">
+        <is>
+          <t>2022-Q1</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="6" t="n">
+        <v>42</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>001651</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>工银瑞信新蓝筹股票A</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>大盘平衡</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>王筱苓</t>
+        </is>
+      </c>
+      <c r="F44" s="8" t="n">
+        <v>42222</v>
+      </c>
+      <c r="G44" s="8" t="n">
+        <v>42222</v>
+      </c>
+      <c r="H44" t="n">
+        <v>5</v>
+      </c>
+      <c r="I44" t="n">
+        <v>5</v>
+      </c>
+      <c r="J44" t="inlineStr">
+        <is>
+          <t>1.27</t>
+        </is>
+      </c>
+      <c r="K44" t="inlineStr">
+        <is>
+          <t>80.99</t>
+        </is>
+      </c>
+      <c r="L44" t="inlineStr">
+        <is>
+          <t>29.29</t>
+        </is>
+      </c>
+      <c r="M44" t="n">
+        <v>2</v>
+      </c>
+      <c r="N44" t="n">
+        <v>2</v>
+      </c>
+      <c r="O44" t="n">
+        <v>3</v>
+      </c>
+      <c r="P44" t="inlineStr">
+        <is>
+          <t>18.04</t>
+        </is>
+      </c>
+      <c r="Q44" t="inlineStr">
+        <is>
+          <t>0.91</t>
+        </is>
+      </c>
+      <c r="R44" t="inlineStr">
+        <is>
+          <t>16.39</t>
+        </is>
+      </c>
+      <c r="S44" t="inlineStr">
+        <is>
+          <t>4.71</t>
+        </is>
+      </c>
+      <c r="T44" t="inlineStr">
+        <is>
+          <t>2022-Q1</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="6" t="n">
+        <v>43</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>000977</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>长城环保主题灵活配置混合</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>大盘成长</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>廖瀚博</t>
+        </is>
+      </c>
+      <c r="F45" s="8" t="n">
+        <v>43167</v>
+      </c>
+      <c r="G45" s="8" t="n">
+        <v>42102</v>
+      </c>
+      <c r="H45" t="n">
+        <v>5</v>
+      </c>
+      <c r="I45" t="n">
+        <v>4</v>
+      </c>
+      <c r="J45" t="inlineStr">
+        <is>
+          <t>1.26</t>
+        </is>
+      </c>
+      <c r="K45" t="inlineStr">
+        <is>
+          <t>81.27</t>
+        </is>
+      </c>
+      <c r="L45" t="inlineStr">
+        <is>
+          <t>37.52</t>
+        </is>
+      </c>
+      <c r="M45" t="n">
+        <v>2</v>
+      </c>
+      <c r="N45" t="n">
+        <v>2</v>
+      </c>
+      <c r="O45" t="n">
+        <v>2</v>
+      </c>
+      <c r="P45" t="inlineStr">
+        <is>
+          <t>25.26</t>
+        </is>
+      </c>
+      <c r="Q45" t="inlineStr">
+        <is>
+          <t>0.96</t>
+        </is>
+      </c>
+      <c r="R45" t="inlineStr">
+        <is>
+          <t>26.01</t>
+        </is>
+      </c>
+      <c r="S45" t="inlineStr">
+        <is>
+          <t>9.63</t>
+        </is>
+      </c>
+      <c r="T45" t="inlineStr">
+        <is>
+          <t>2022-Q1</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="6" t="n">
+        <v>44</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>001487</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>宝盈优势产业灵活配置混合</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>中盘成长</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>陈金伟</t>
+        </is>
+      </c>
+      <c r="F46" s="8" t="n">
+        <v>44202</v>
+      </c>
+      <c r="G46" s="8" t="n">
+        <v>42241</v>
+      </c>
+      <c r="H46" t="n">
+        <v>5</v>
+      </c>
+      <c r="I46" t="n">
+        <v>5</v>
+      </c>
+      <c r="J46" t="inlineStr">
+        <is>
+          <t>1.25</t>
+        </is>
+      </c>
+      <c r="K46" t="inlineStr">
+        <is>
+          <t>91.61</t>
+        </is>
+      </c>
+      <c r="L46" t="inlineStr">
+        <is>
+          <t>33.56</t>
+        </is>
+      </c>
+      <c r="M46" t="n">
+        <v>2</v>
+      </c>
+      <c r="N46" t="n">
+        <v>2</v>
+      </c>
+      <c r="O46" t="n">
+        <v>2</v>
+      </c>
+      <c r="P46" t="inlineStr">
+        <is>
+          <t>25.80</t>
+        </is>
+      </c>
+      <c r="Q46" t="inlineStr">
+        <is>
+          <t>0.57</t>
+        </is>
+      </c>
+      <c r="R46" t="inlineStr">
+        <is>
+          <t>24.18</t>
+        </is>
+      </c>
+      <c r="S46" t="inlineStr">
+        <is>
+          <t>17.02</t>
+        </is>
+      </c>
+      <c r="T46" t="inlineStr">
+        <is>
+          <t>2022-Q1</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="6" t="n">
+        <v>45</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>002133</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>广发鑫益灵活配置混合</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>大盘成长</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>费逸</t>
+        </is>
+      </c>
+      <c r="F47" s="8" t="n">
+        <v>43314</v>
+      </c>
+      <c r="G47" s="8" t="n">
+        <v>42690</v>
+      </c>
+      <c r="H47" t="n">
+        <v>5</v>
+      </c>
+      <c r="I47" t="n">
+        <v>4</v>
+      </c>
+      <c r="J47" t="inlineStr">
+        <is>
+          <t>1.25</t>
+        </is>
+      </c>
+      <c r="K47" t="inlineStr">
+        <is>
+          <t>88.17</t>
+        </is>
+      </c>
+      <c r="L47" t="inlineStr">
+        <is>
+          <t>46.49</t>
+        </is>
+      </c>
+      <c r="M47" t="n">
+        <v>2</v>
+      </c>
+      <c r="N47" t="n">
+        <v>2</v>
+      </c>
+      <c r="O47" t="n">
+        <v>2</v>
+      </c>
+      <c r="P47" t="inlineStr">
+        <is>
+          <t>20.93</t>
+        </is>
+      </c>
+      <c r="Q47" t="inlineStr">
+        <is>
+          <t>1.84</t>
+        </is>
+      </c>
+      <c r="R47" t="inlineStr">
+        <is>
+          <t>21.62</t>
+        </is>
+      </c>
+      <c r="S47" t="inlineStr">
+        <is>
+          <t>2.84</t>
+        </is>
+      </c>
+      <c r="T47" t="inlineStr">
+        <is>
+          <t>2022-Q1</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="6" t="n">
+        <v>46</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>000263</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>工银瑞信信息产业混合A</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>大盘成长</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>单文</t>
+        </is>
+      </c>
+      <c r="F48" s="8" t="n">
+        <v>42941</v>
+      </c>
+      <c r="G48" s="8" t="n">
+        <v>41589</v>
+      </c>
+      <c r="H48" t="n">
+        <v>5</v>
+      </c>
+      <c r="I48" t="n">
+        <v>5</v>
+      </c>
+      <c r="J48" t="inlineStr">
+        <is>
+          <t>1.23</t>
+        </is>
+      </c>
+      <c r="K48" t="inlineStr">
+        <is>
+          <t>83.76</t>
+        </is>
+      </c>
+      <c r="L48" t="inlineStr">
+        <is>
+          <t>35.10</t>
+        </is>
+      </c>
+      <c r="M48" t="n">
+        <v>3</v>
+      </c>
+      <c r="N48" t="n">
+        <v>4</v>
+      </c>
+      <c r="O48" t="n">
+        <v>4</v>
+      </c>
+      <c r="P48" t="inlineStr">
+        <is>
+          <t>27.26</t>
+        </is>
+      </c>
+      <c r="Q48" t="inlineStr">
+        <is>
+          <t>0.78</t>
+        </is>
+      </c>
+      <c r="R48" t="inlineStr">
+        <is>
+          <t>24.62</t>
+        </is>
+      </c>
+      <c r="S48" t="inlineStr">
+        <is>
+          <t>27.45</t>
+        </is>
+      </c>
+      <c r="T48" t="inlineStr">
+        <is>
+          <t>2022-Q1</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="6" t="n">
+        <v>47</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>001276</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>建信新经济灵活配置混合</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>大盘成长</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>孙晟</t>
+        </is>
+      </c>
+      <c r="F49" s="8" t="n">
+        <v>44029</v>
+      </c>
+      <c r="G49" s="8" t="n">
+        <v>42150</v>
+      </c>
+      <c r="H49" t="n">
+        <v>5</v>
+      </c>
+      <c r="I49" t="n">
+        <v>4</v>
+      </c>
+      <c r="J49" t="inlineStr">
+        <is>
+          <t>1.23</t>
+        </is>
+      </c>
+      <c r="K49" t="inlineStr">
+        <is>
+          <t>84.07</t>
+        </is>
+      </c>
+      <c r="L49" t="inlineStr">
+        <is>
+          <t>58.66</t>
+        </is>
+      </c>
+      <c r="M49" t="n">
+        <v>3</v>
+      </c>
+      <c r="N49" t="n">
+        <v>3</v>
+      </c>
+      <c r="O49" t="n">
+        <v>2</v>
+      </c>
+      <c r="P49" t="inlineStr">
+        <is>
+          <t>19.04</t>
+        </is>
+      </c>
+      <c r="Q49" t="inlineStr">
+        <is>
+          <t>1.66</t>
+        </is>
+      </c>
+      <c r="R49" t="inlineStr">
+        <is>
+          <t>19.95</t>
+        </is>
+      </c>
+      <c r="S49" t="inlineStr">
+        <is>
+          <t>1.59</t>
+        </is>
+      </c>
+      <c r="T49" t="inlineStr">
+        <is>
+          <t>2022-Q1</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="6" t="n">
+        <v>48</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>001208</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>诺安低碳经济股票A</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>大盘平衡</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>蔡宇滨</t>
+        </is>
+      </c>
+      <c r="F50" s="8" t="n">
+        <v>43487</v>
+      </c>
+      <c r="G50" s="8" t="n">
+        <v>42136</v>
+      </c>
+      <c r="H50" t="n">
+        <v>5</v>
+      </c>
+      <c r="I50" t="n">
+        <v>5</v>
+      </c>
+      <c r="J50" t="inlineStr">
+        <is>
+          <t>1.22</t>
+        </is>
+      </c>
+      <c r="K50" t="inlineStr">
+        <is>
+          <t>82.03</t>
+        </is>
+      </c>
+      <c r="L50" t="inlineStr">
+        <is>
+          <t>30.18</t>
+        </is>
+      </c>
+      <c r="M50" t="n">
+        <v>4</v>
+      </c>
+      <c r="N50" t="n">
+        <v>3</v>
+      </c>
+      <c r="O50" t="n">
+        <v>3</v>
+      </c>
+      <c r="P50" t="inlineStr">
+        <is>
+          <t>16.78</t>
+        </is>
+      </c>
+      <c r="Q50" t="inlineStr">
+        <is>
+          <t>0.73</t>
+        </is>
+      </c>
+      <c r="R50" t="inlineStr">
+        <is>
+          <t>15.58</t>
+        </is>
+      </c>
+      <c r="S50" t="inlineStr">
+        <is>
+          <t>14.51</t>
+        </is>
+      </c>
+      <c r="T50" t="inlineStr">
+        <is>
+          <t>2022-Q1</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="6" t="n">
+        <v>49</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>000541</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>华商创新成长灵活配置混合</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>大盘成长</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>梁皓</t>
+        </is>
+      </c>
+      <c r="F51" s="8" t="n">
+        <v>43293</v>
+      </c>
+      <c r="G51" s="8" t="n">
+        <v>41716</v>
+      </c>
+      <c r="H51" t="n">
+        <v>5</v>
+      </c>
+      <c r="I51" t="n">
+        <v>3</v>
+      </c>
+      <c r="J51" t="inlineStr">
+        <is>
+          <t>1.21</t>
+        </is>
+      </c>
+      <c r="K51" t="inlineStr">
+        <is>
+          <t>87.52</t>
+        </is>
+      </c>
+      <c r="L51" t="inlineStr">
+        <is>
+          <t>48.43</t>
+        </is>
+      </c>
+      <c r="M51" t="n">
+        <v>2</v>
+      </c>
+      <c r="N51" t="n">
+        <v>2</v>
+      </c>
+      <c r="O51" t="n">
+        <v>2</v>
+      </c>
+      <c r="P51" t="inlineStr">
+        <is>
+          <t>24.72</t>
+        </is>
+      </c>
+      <c r="Q51" t="inlineStr">
+        <is>
+          <t>0.85</t>
+        </is>
+      </c>
+      <c r="R51" t="inlineStr">
+        <is>
+          <t>25.93</t>
+        </is>
+      </c>
+      <c r="S51" t="inlineStr">
+        <is>
+          <t>7.86</t>
+        </is>
+      </c>
+      <c r="T51" t="inlineStr">
+        <is>
+          <t>2022-Q1</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="6" t="n">
+        <v>50</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>001171</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>工银瑞信养老产业股票</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>大盘成长</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>赵蓓</t>
+        </is>
+      </c>
+      <c r="F52" s="8" t="n">
+        <v>42122</v>
+      </c>
+      <c r="G52" s="8" t="n">
+        <v>42122</v>
+      </c>
+      <c r="H52" t="n">
+        <v>5</v>
+      </c>
+      <c r="I52" t="n">
+        <v>5</v>
+      </c>
+      <c r="J52" t="inlineStr">
+        <is>
+          <t>1.20</t>
+        </is>
+      </c>
+      <c r="K52" t="inlineStr">
+        <is>
+          <t>82.83</t>
+        </is>
+      </c>
+      <c r="L52" t="inlineStr">
+        <is>
+          <t>49.58</t>
+        </is>
+      </c>
+      <c r="M52" t="n">
+        <v>3</v>
+      </c>
+      <c r="N52" t="n">
+        <v>3</v>
+      </c>
+      <c r="O52" t="n">
+        <v>3</v>
+      </c>
+      <c r="P52" t="inlineStr">
+        <is>
+          <t>23.59</t>
+        </is>
+      </c>
+      <c r="Q52" t="inlineStr">
+        <is>
+          <t>0.87</t>
+        </is>
+      </c>
+      <c r="R52" t="inlineStr">
+        <is>
+          <t>24.43</t>
+        </is>
+      </c>
+      <c r="S52" t="inlineStr">
+        <is>
+          <t>37.09</t>
+        </is>
+      </c>
+      <c r="T52" t="inlineStr">
+        <is>
+          <t>2022-Q1</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="6" t="n">
+        <v>51</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>070027</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>嘉实周期优选混合</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>大盘价值</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>肖觅</t>
+        </is>
+      </c>
+      <c r="F53" s="8" t="n">
+        <v>43987</v>
+      </c>
+      <c r="G53" s="8" t="n">
+        <v>40885</v>
+      </c>
+      <c r="H53" t="n">
+        <v>5</v>
+      </c>
+      <c r="I53" t="n">
+        <v>3</v>
+      </c>
+      <c r="J53" t="inlineStr">
+        <is>
+          <t>1.20</t>
+        </is>
+      </c>
+      <c r="K53" t="inlineStr">
+        <is>
+          <t>90.55</t>
+        </is>
+      </c>
+      <c r="L53" t="inlineStr">
+        <is>
+          <t>56.19</t>
+        </is>
+      </c>
+      <c r="M53" t="n">
+        <v>4</v>
+      </c>
+      <c r="N53" t="n">
+        <v>2</v>
+      </c>
+      <c r="O53" t="n">
+        <v>2</v>
+      </c>
+      <c r="P53" t="inlineStr">
+        <is>
+          <t>18.81</t>
+        </is>
+      </c>
+      <c r="Q53" t="inlineStr">
+        <is>
+          <t>0.86</t>
+        </is>
+      </c>
+      <c r="R53" t="inlineStr">
+        <is>
+          <t>17.89</t>
+        </is>
+      </c>
+      <c r="S53" t="inlineStr">
+        <is>
+          <t>8.84</t>
+        </is>
+      </c>
+      <c r="T53" t="inlineStr">
+        <is>
+          <t>2022-Q1</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="6" t="n">
+        <v>52</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>001220</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>民生加银研究精选灵活配置混合</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>大盘成长</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>蔡晓</t>
+        </is>
+      </c>
+      <c r="F54" s="8" t="n">
+        <v>43166</v>
+      </c>
+      <c r="G54" s="8" t="n">
+        <v>42151</v>
+      </c>
+      <c r="H54" t="n">
+        <v>5</v>
+      </c>
+      <c r="I54" t="n">
+        <v>4</v>
+      </c>
+      <c r="J54" t="inlineStr">
+        <is>
+          <t>1.19</t>
+        </is>
+      </c>
+      <c r="K54" t="inlineStr">
+        <is>
+          <t>92.72</t>
+        </is>
+      </c>
+      <c r="L54" t="inlineStr">
+        <is>
+          <t>39.27</t>
+        </is>
+      </c>
+      <c r="M54" t="n">
+        <v>2</v>
+      </c>
+      <c r="N54" t="n">
+        <v>2</v>
+      </c>
+      <c r="O54" t="n">
+        <v>2</v>
+      </c>
+      <c r="P54" t="inlineStr">
+        <is>
+          <t>21.81</t>
+        </is>
+      </c>
+      <c r="Q54" t="inlineStr">
+        <is>
+          <t>1.76</t>
+        </is>
+      </c>
+      <c r="R54" t="inlineStr">
+        <is>
+          <t>23.21</t>
+        </is>
+      </c>
+      <c r="S54" t="inlineStr">
+        <is>
+          <t>2.66</t>
+        </is>
+      </c>
+      <c r="T54" t="inlineStr">
+        <is>
+          <t>2022-Q1</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="6" t="n">
+        <v>53</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>000339</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>长城医疗保健混合</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>中盘成长</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>谭小兵</t>
+        </is>
+      </c>
+      <c r="F55" s="8" t="n">
+        <v>42403</v>
+      </c>
+      <c r="G55" s="8" t="n">
+        <v>41698</v>
+      </c>
+      <c r="H55" t="n">
+        <v>5</v>
+      </c>
+      <c r="I55" t="n">
+        <v>5</v>
+      </c>
+      <c r="J55" t="inlineStr">
+        <is>
+          <t>1.09</t>
+        </is>
+      </c>
+      <c r="K55" t="inlineStr">
+        <is>
+          <t>88.40</t>
+        </is>
+      </c>
+      <c r="L55" t="inlineStr">
+        <is>
+          <t>40.83</t>
+        </is>
+      </c>
+      <c r="M55" t="n">
+        <v>4</v>
+      </c>
+      <c r="N55" t="n">
+        <v>4</v>
+      </c>
+      <c r="O55" t="n">
+        <v>4</v>
+      </c>
+      <c r="P55" t="inlineStr">
+        <is>
+          <t>20.90</t>
+        </is>
+      </c>
+      <c r="Q55" t="inlineStr">
+        <is>
+          <t>0.92</t>
+        </is>
+      </c>
+      <c r="R55" t="inlineStr">
+        <is>
+          <t>24.88</t>
+        </is>
+      </c>
+      <c r="S55" t="inlineStr">
+        <is>
+          <t>11.06</t>
+        </is>
+      </c>
+      <c r="T55" t="inlineStr">
+        <is>
+          <t>2022-Q1</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="6" t="n">
+        <v>54</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>519171</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>浦银安盛医疗健康灵活配置混合</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>大盘成长</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>胡攸乔</t>
+        </is>
+      </c>
+      <c r="F56" s="8" t="n">
+        <v>44168</v>
+      </c>
+      <c r="G56" s="8" t="n">
+        <v>42149</v>
+      </c>
+      <c r="H56" t="n">
+        <v>5</v>
+      </c>
+      <c r="I56" t="n">
+        <v>4</v>
+      </c>
+      <c r="J56" t="inlineStr">
+        <is>
+          <t>1.07</t>
+        </is>
+      </c>
+      <c r="K56" t="inlineStr">
+        <is>
+          <t>88.21</t>
+        </is>
+      </c>
+      <c r="L56" t="inlineStr">
+        <is>
+          <t>41.65</t>
+        </is>
+      </c>
+      <c r="M56" t="n">
+        <v>2</v>
+      </c>
+      <c r="N56" t="n">
+        <v>3</v>
+      </c>
+      <c r="O56" t="n">
+        <v>3</v>
+      </c>
+      <c r="P56" t="inlineStr">
+        <is>
+          <t>21.96</t>
+        </is>
+      </c>
+      <c r="Q56" t="inlineStr">
+        <is>
+          <t>1.02</t>
+        </is>
+      </c>
+      <c r="R56" t="inlineStr">
+        <is>
+          <t>27.08</t>
+        </is>
+      </c>
+      <c r="S56" t="inlineStr">
+        <is>
+          <t>15.50</t>
+        </is>
+      </c>
+      <c r="T56" t="inlineStr">
+        <is>
+          <t>2022-Q1</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="6" t="n">
+        <v>55</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>000831</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>工银瑞信医疗保健行业股票</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>大盘成长</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>赵蓓</t>
+        </is>
+      </c>
+      <c r="F57" s="8" t="n">
+        <v>41961</v>
+      </c>
+      <c r="G57" s="8" t="n">
+        <v>41961</v>
+      </c>
+      <c r="H57" t="n">
+        <v>5</v>
+      </c>
+      <c r="I57" t="n">
+        <v>4</v>
+      </c>
+      <c r="J57" t="inlineStr">
+        <is>
+          <t>1.03</t>
+        </is>
+      </c>
+      <c r="K57" t="inlineStr">
+        <is>
+          <t>82.75</t>
+        </is>
+      </c>
+      <c r="L57" t="inlineStr">
+        <is>
+          <t>52.51</t>
+        </is>
+      </c>
+      <c r="M57" t="n">
+        <v>2</v>
+      </c>
+      <c r="N57" t="n">
+        <v>2</v>
+      </c>
+      <c r="O57" t="n">
+        <v>2</v>
+      </c>
+      <c r="P57" t="inlineStr">
+        <is>
+          <t>21.50</t>
+        </is>
+      </c>
+      <c r="Q57" t="inlineStr">
+        <is>
+          <t>0.99</t>
+        </is>
+      </c>
+      <c r="R57" t="inlineStr">
+        <is>
+          <t>27.34</t>
+        </is>
+      </c>
+      <c r="S57" t="inlineStr">
+        <is>
+          <t>44.04</t>
+        </is>
+      </c>
+      <c r="T57" t="inlineStr">
+        <is>
+          <t>2022-Q1</t>
         </is>
       </c>
     </row>

</xml_diff>